<commit_message>
Add ability for pathfinders to stand on corners of each cell when assessing if they can fit somewhere.
</commit_message>
<xml_diff>
--- a/csharp_pathfinding/AStarTests/Resources/excel_mazes/walls.xlsx
+++ b/csharp_pathfinding/AStarTests/Resources/excel_mazes/walls.xlsx
@@ -206,10 +206,10 @@
   <dimension ref="A1:BV44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AR19" activeCellId="0" sqref="AR19"/>
+      <selection pane="topLeft" activeCell="AN4" activeCellId="0" sqref="AN4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5625" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="AN3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="1" t="n">
         <v>1</v>
@@ -926,7 +926,7 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="1" t="n">
         <v>1</v>

</xml_diff>